<commit_message>
silence analysis tab for now
</commit_message>
<xml_diff>
--- a/test_data/Design.xlsx
+++ b/test_data/Design.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10720"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danmarti/Documents/MRC_postdoc/Utils/cell_growth/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB642E8-386B-784E-9C68-E5D9BCE6DF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69EEB67-DC2B-4543-BB8B-9CB9DEAAFC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="1800" windowWidth="25280" windowHeight="17860" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="1" r:id="rId1"/>
-    <sheet name="analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="_analysis" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Design!$A$1:$E$1</definedName>

</xml_diff>